<commit_message>
update the doc for reg to apb2
</commit_message>
<xml_diff>
--- a/doc/uvm_mcdf_env.xlsx
+++ b/doc/uvm_mcdf_env.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="137">
   <si>
     <t>MCDF</t>
   </si>
@@ -468,51 +468,30 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
+    <t>总线选择</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>pwr_i</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>写标识</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>待操作地址</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>pen_i</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
     <t>1bit</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>总线选择</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>pwr_i</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>写标识</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>待操作地址</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>pready_o</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>读或写操作完成标识</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>总线操作错误（例如无效空间访问）</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>register
-(APB Bus)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>pen_i</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>1bit</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>总线使能</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -533,7 +512,8 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>pslverr_o</t>
+    <t>register
+(APB2 Bus)</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1279,47 +1259,71 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1339,17 +1343,92 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1448,105 +1527,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1897,10 +1877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Z36"/>
+  <dimension ref="B1:Z34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W27" sqref="W27"/>
+      <selection activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="16.8"/>
@@ -1936,10 +1916,10 @@
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="2:26" ht="18.600000000000001">
-      <c r="B2" s="171" t="s">
+      <c r="B2" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="97" t="s">
+      <c r="C2" s="84" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -1974,8 +1954,8 @@
       <c r="Z2" s="21"/>
     </row>
     <row r="3" spans="2:26" ht="18.600000000000001">
-      <c r="B3" s="172"/>
-      <c r="C3" s="97"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="84"/>
       <c r="D3" s="8" t="s">
         <v>2</v>
       </c>
@@ -1989,43 +1969,43 @@
         <v>7</v>
       </c>
       <c r="I3" s="21"/>
-      <c r="J3" s="84" t="s">
+      <c r="J3" s="85" t="s">
         <v>8</v>
       </c>
       <c r="K3" s="24"/>
-      <c r="L3" s="84" t="s">
+      <c r="L3" s="85" t="s">
         <v>9</v>
       </c>
       <c r="M3" s="24"/>
-      <c r="N3" s="84" t="s">
+      <c r="N3" s="85" t="s">
         <v>10</v>
       </c>
       <c r="O3" s="24"/>
-      <c r="P3" s="84" t="s">
+      <c r="P3" s="85" t="s">
         <v>11</v>
       </c>
       <c r="Q3" s="24"/>
-      <c r="R3" s="84" t="s">
+      <c r="R3" s="85" t="s">
         <v>12</v>
       </c>
       <c r="S3" s="24"/>
-      <c r="T3" s="84" t="s">
+      <c r="T3" s="85" t="s">
         <v>13</v>
       </c>
       <c r="U3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="V3" s="88" t="s">
+      <c r="V3" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="W3" s="89"/>
+      <c r="W3" s="93"/>
       <c r="X3" s="21"/>
       <c r="Y3" s="26"/>
       <c r="Z3" s="21"/>
     </row>
     <row r="4" spans="2:26" ht="18.600000000000001">
-      <c r="B4" s="172"/>
-      <c r="C4" s="94" t="s">
+      <c r="B4" s="90"/>
+      <c r="C4" s="98" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="10" t="s">
@@ -2041,27 +2021,27 @@
         <v>18</v>
       </c>
       <c r="I4" s="21"/>
-      <c r="J4" s="85"/>
+      <c r="J4" s="86"/>
       <c r="K4" s="25"/>
-      <c r="L4" s="85"/>
+      <c r="L4" s="86"/>
       <c r="M4" s="25"/>
-      <c r="N4" s="85"/>
+      <c r="N4" s="86"/>
       <c r="O4" s="25"/>
-      <c r="P4" s="85"/>
+      <c r="P4" s="86"/>
       <c r="Q4" s="25"/>
-      <c r="R4" s="85"/>
+      <c r="R4" s="86"/>
       <c r="S4" s="25"/>
-      <c r="T4" s="85"/>
+      <c r="T4" s="86"/>
       <c r="U4" s="21"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="91"/>
+      <c r="V4" s="94"/>
+      <c r="W4" s="95"/>
       <c r="X4" s="21"/>
       <c r="Y4" s="26"/>
       <c r="Z4" s="21"/>
     </row>
     <row r="5" spans="2:26" ht="18.600000000000001">
-      <c r="B5" s="172"/>
-      <c r="C5" s="94"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="98"/>
       <c r="D5" s="10" t="s">
         <v>2</v>
       </c>
@@ -2087,8 +2067,8 @@
       <c r="S5" s="26"/>
       <c r="T5" s="26"/>
       <c r="U5" s="21"/>
-      <c r="V5" s="90"/>
-      <c r="W5" s="91"/>
+      <c r="V5" s="94"/>
+      <c r="W5" s="95"/>
       <c r="X5" s="21"/>
       <c r="Y5" s="28" t="s">
         <v>22</v>
@@ -2096,8 +2076,8 @@
       <c r="Z5" s="21"/>
     </row>
     <row r="6" spans="2:26" ht="18.600000000000001">
-      <c r="B6" s="172"/>
-      <c r="C6" s="94"/>
+      <c r="B6" s="90"/>
+      <c r="C6" s="98"/>
       <c r="D6" s="10" t="s">
         <v>2</v>
       </c>
@@ -2123,8 +2103,8 @@
       <c r="S6" s="26"/>
       <c r="T6" s="26"/>
       <c r="U6" s="21"/>
-      <c r="V6" s="90"/>
-      <c r="W6" s="91"/>
+      <c r="V6" s="94"/>
+      <c r="W6" s="95"/>
       <c r="X6" s="21"/>
       <c r="Y6" s="28" t="s">
         <v>25</v>
@@ -2132,8 +2112,8 @@
       <c r="Z6" s="21"/>
     </row>
     <row r="7" spans="2:26" ht="18.600000000000001">
-      <c r="B7" s="172"/>
-      <c r="C7" s="95" t="s">
+      <c r="B7" s="90"/>
+      <c r="C7" s="99" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="12" t="s">
@@ -2149,34 +2129,34 @@
         <v>75</v>
       </c>
       <c r="I7" s="21"/>
-      <c r="J7" s="84" t="s">
+      <c r="J7" s="85" t="s">
         <v>8</v>
       </c>
       <c r="K7" s="24"/>
-      <c r="L7" s="84" t="s">
+      <c r="L7" s="85" t="s">
         <v>9</v>
       </c>
       <c r="M7" s="24"/>
-      <c r="N7" s="84" t="s">
+      <c r="N7" s="85" t="s">
         <v>10</v>
       </c>
       <c r="O7" s="24"/>
-      <c r="P7" s="84" t="s">
+      <c r="P7" s="85" t="s">
         <v>11</v>
       </c>
       <c r="Q7" s="24"/>
-      <c r="R7" s="84" t="s">
+      <c r="R7" s="85" t="s">
         <v>12</v>
       </c>
       <c r="S7" s="24"/>
-      <c r="T7" s="84" t="s">
+      <c r="T7" s="85" t="s">
         <v>13</v>
       </c>
       <c r="U7" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="V7" s="90"/>
-      <c r="W7" s="91"/>
+      <c r="V7" s="94"/>
+      <c r="W7" s="95"/>
       <c r="X7" s="21"/>
       <c r="Y7" s="28" t="s">
         <v>8</v>
@@ -2184,8 +2164,8 @@
       <c r="Z7" s="21"/>
     </row>
     <row r="8" spans="2:26" ht="18.600000000000001">
-      <c r="B8" s="172"/>
-      <c r="C8" s="95"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="99"/>
       <c r="D8" s="12" t="s">
         <v>2</v>
       </c>
@@ -2199,20 +2179,20 @@
         <v>75</v>
       </c>
       <c r="I8" s="21"/>
-      <c r="J8" s="85"/>
+      <c r="J8" s="86"/>
       <c r="K8" s="25"/>
-      <c r="L8" s="85"/>
+      <c r="L8" s="86"/>
       <c r="M8" s="25"/>
-      <c r="N8" s="85"/>
+      <c r="N8" s="86"/>
       <c r="O8" s="25"/>
-      <c r="P8" s="85"/>
+      <c r="P8" s="86"/>
       <c r="Q8" s="25"/>
-      <c r="R8" s="85"/>
+      <c r="R8" s="86"/>
       <c r="S8" s="25"/>
-      <c r="T8" s="85"/>
+      <c r="T8" s="86"/>
       <c r="U8" s="21"/>
-      <c r="V8" s="90"/>
-      <c r="W8" s="91"/>
+      <c r="V8" s="94"/>
+      <c r="W8" s="95"/>
       <c r="X8" s="23"/>
       <c r="Y8" s="28" t="s">
         <v>9</v>
@@ -2220,8 +2200,8 @@
       <c r="Z8" s="21"/>
     </row>
     <row r="9" spans="2:26" ht="18.600000000000001">
-      <c r="B9" s="172"/>
-      <c r="C9" s="95"/>
+      <c r="B9" s="90"/>
+      <c r="C9" s="99"/>
       <c r="D9" s="12" t="s">
         <v>2</v>
       </c>
@@ -2247,8 +2227,8 @@
       <c r="S9" s="26"/>
       <c r="T9" s="26"/>
       <c r="U9" s="21"/>
-      <c r="V9" s="90"/>
-      <c r="W9" s="91"/>
+      <c r="V9" s="94"/>
+      <c r="W9" s="95"/>
       <c r="X9" s="21"/>
       <c r="Y9" s="28" t="s">
         <v>10</v>
@@ -2256,8 +2236,8 @@
       <c r="Z9" s="21"/>
     </row>
     <row r="10" spans="2:26" ht="18.600000000000001">
-      <c r="B10" s="172"/>
-      <c r="C10" s="96" t="s">
+      <c r="B10" s="90"/>
+      <c r="C10" s="100" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="14" t="s">
@@ -2285,8 +2265,8 @@
       <c r="S10" s="26"/>
       <c r="T10" s="26"/>
       <c r="U10" s="21"/>
-      <c r="V10" s="90"/>
-      <c r="W10" s="91"/>
+      <c r="V10" s="94"/>
+      <c r="W10" s="95"/>
       <c r="X10" s="21"/>
       <c r="Y10" s="28" t="s">
         <v>11</v>
@@ -2294,8 +2274,8 @@
       <c r="Z10" s="21"/>
     </row>
     <row r="11" spans="2:26" ht="18.600000000000001">
-      <c r="B11" s="172"/>
-      <c r="C11" s="96"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="100"/>
       <c r="D11" s="14" t="s">
         <v>2</v>
       </c>
@@ -2309,34 +2289,34 @@
         <v>75</v>
       </c>
       <c r="I11" s="21"/>
-      <c r="J11" s="84" t="s">
+      <c r="J11" s="85" t="s">
         <v>8</v>
       </c>
       <c r="K11" s="24"/>
-      <c r="L11" s="84" t="s">
+      <c r="L11" s="85" t="s">
         <v>9</v>
       </c>
       <c r="M11" s="24"/>
-      <c r="N11" s="84" t="s">
+      <c r="N11" s="85" t="s">
         <v>10</v>
       </c>
       <c r="O11" s="24"/>
-      <c r="P11" s="84" t="s">
+      <c r="P11" s="85" t="s">
         <v>11</v>
       </c>
       <c r="Q11" s="24"/>
-      <c r="R11" s="84" t="s">
+      <c r="R11" s="85" t="s">
         <v>12</v>
       </c>
       <c r="S11" s="24"/>
-      <c r="T11" s="84" t="s">
+      <c r="T11" s="85" t="s">
         <v>13</v>
       </c>
       <c r="U11" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="V11" s="90"/>
-      <c r="W11" s="91"/>
+      <c r="V11" s="94"/>
+      <c r="W11" s="95"/>
       <c r="X11" s="21"/>
       <c r="Y11" s="28" t="s">
         <v>35</v>
@@ -2344,8 +2324,8 @@
       <c r="Z11" s="21"/>
     </row>
     <row r="12" spans="2:26" ht="18.600000000000001">
-      <c r="B12" s="172"/>
-      <c r="C12" s="96"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="100"/>
       <c r="D12" s="14" t="s">
         <v>2</v>
       </c>
@@ -2359,20 +2339,20 @@
         <v>75</v>
       </c>
       <c r="I12" s="21"/>
-      <c r="J12" s="85"/>
+      <c r="J12" s="86"/>
       <c r="K12" s="25"/>
-      <c r="L12" s="85"/>
+      <c r="L12" s="86"/>
       <c r="M12" s="25"/>
-      <c r="N12" s="85"/>
+      <c r="N12" s="86"/>
       <c r="O12" s="25"/>
-      <c r="P12" s="85"/>
+      <c r="P12" s="86"/>
       <c r="Q12" s="25"/>
-      <c r="R12" s="85"/>
+      <c r="R12" s="86"/>
       <c r="S12" s="25"/>
-      <c r="T12" s="85"/>
+      <c r="T12" s="86"/>
       <c r="U12" s="21"/>
-      <c r="V12" s="90"/>
-      <c r="W12" s="91"/>
+      <c r="V12" s="94"/>
+      <c r="W12" s="95"/>
       <c r="X12" s="21"/>
       <c r="Y12" s="28" t="s">
         <v>37</v>
@@ -2380,8 +2360,8 @@
       <c r="Z12" s="21"/>
     </row>
     <row r="13" spans="2:26" ht="18.600000000000001">
-      <c r="B13" s="172"/>
-      <c r="C13" s="86" t="s">
+      <c r="B13" s="90"/>
+      <c r="C13" s="101" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="16" t="s">
@@ -2409,15 +2389,15 @@
       <c r="S13" s="21"/>
       <c r="T13" s="21"/>
       <c r="U13" s="21"/>
-      <c r="V13" s="92"/>
-      <c r="W13" s="93"/>
+      <c r="V13" s="96"/>
+      <c r="W13" s="97"/>
       <c r="X13" s="21"/>
       <c r="Y13" s="26"/>
       <c r="Z13" s="21"/>
     </row>
     <row r="14" spans="2:26" ht="18.600000000000001">
-      <c r="B14" s="172"/>
-      <c r="C14" s="86"/>
+      <c r="B14" s="90"/>
+      <c r="C14" s="101"/>
       <c r="D14" s="16" t="s">
         <v>16</v>
       </c>
@@ -2450,8 +2430,8 @@
       <c r="Z14" s="21"/>
     </row>
     <row r="15" spans="2:26" ht="18.600000000000001">
-      <c r="B15" s="172"/>
-      <c r="C15" s="86"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="101"/>
       <c r="D15" s="16" t="s">
         <v>16</v>
       </c>
@@ -2466,8 +2446,8 @@
       </c>
     </row>
     <row r="16" spans="2:26" ht="18.600000000000001">
-      <c r="B16" s="172"/>
-      <c r="C16" s="86"/>
+      <c r="B16" s="90"/>
+      <c r="C16" s="101"/>
       <c r="D16" s="16" t="s">
         <v>2</v>
       </c>
@@ -2482,8 +2462,8 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="18.600000000000001">
-      <c r="B17" s="172"/>
-      <c r="C17" s="86"/>
+      <c r="B17" s="90"/>
+      <c r="C17" s="101"/>
       <c r="D17" s="16" t="s">
         <v>16</v>
       </c>
@@ -2498,8 +2478,8 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="18.600000000000001">
-      <c r="B18" s="172"/>
-      <c r="C18" s="86"/>
+      <c r="B18" s="90"/>
+      <c r="C18" s="101"/>
       <c r="D18" s="16" t="s">
         <v>16</v>
       </c>
@@ -2514,8 +2494,8 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="18.600000000000001">
-      <c r="B19" s="172"/>
-      <c r="C19" s="86"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="101"/>
       <c r="D19" s="16" t="s">
         <v>16</v>
       </c>
@@ -2530,79 +2510,79 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="18.600000000000001" customHeight="1">
-      <c r="B20" s="172"/>
-      <c r="C20" s="170" t="s">
-        <v>133</v>
+      <c r="B20" s="90"/>
+      <c r="C20" s="87" t="s">
+        <v>136</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F20" s="31" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="G20" s="32" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="18.600000000000001">
-      <c r="B21" s="172"/>
-      <c r="C21" s="170"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="87"/>
       <c r="D21" s="18" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="18.600000000000001">
-      <c r="B22" s="172"/>
-      <c r="C22" s="170"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="87"/>
       <c r="D22" s="18" t="s">
         <v>2</v>
       </c>
       <c r="E22" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="G22" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="F22" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="G22" s="32" t="s">
-        <v>128</v>
-      </c>
     </row>
     <row r="23" spans="2:7" ht="18.600000000000001">
-      <c r="B23" s="172"/>
-      <c r="C23" s="170"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="87"/>
       <c r="D23" s="18" t="s">
         <v>2</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F23" s="31" t="s">
         <v>52</v>
       </c>
       <c r="G23" s="32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="18.600000000000001">
-      <c r="B24" s="172"/>
-      <c r="C24" s="87"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="88"/>
       <c r="D24" s="18" t="s">
         <v>2</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F24" s="31" t="s">
         <v>20</v>
@@ -2612,66 +2592,33 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="18.600000000000001">
-      <c r="B25" s="172"/>
-      <c r="C25" s="87"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="88"/>
       <c r="D25" s="18" t="s">
         <v>16</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="F25" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="F25" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="32" t="s">
+      <c r="G25" s="34" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="18.600000000000001">
-      <c r="B26" s="172"/>
-      <c r="C26" s="87"/>
-      <c r="D26" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="F26" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="G26" s="32" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="18.600000000000001">
-      <c r="B27" s="173"/>
-      <c r="C27" s="87"/>
-      <c r="D27" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="F27" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="G27" s="34" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="22.8" customHeight="1"/>
-    <row r="36" spans="2:3">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+    <row r="26" spans="2:7" ht="22.8" customHeight="1"/>
+    <row r="34" spans="2:3">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="C20:C27"/>
-    <mergeCell ref="B2:B27"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="T11:T12"/>
+    <mergeCell ref="C13:C19"/>
+    <mergeCell ref="B2:B25"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="T3:T4"/>
@@ -2687,11 +2634,12 @@
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="L11:L12"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="C20:C25"/>
     <mergeCell ref="N11:N12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="T11:T12"/>
-    <mergeCell ref="C13:C19"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -2738,13 +2686,13 @@
       </c>
     </row>
     <row r="3" spans="2:6" ht="22.8" customHeight="1">
-      <c r="B3" s="101" t="s">
+      <c r="B3" s="109" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="98" t="s">
+      <c r="C3" s="106" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="98" t="s">
+      <c r="D3" s="106" t="s">
         <v>85</v>
       </c>
       <c r="E3" s="36" t="s">
@@ -2755,9 +2703,9 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="22.8">
-      <c r="B4" s="102"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="107"/>
       <c r="E4" s="36" t="s">
         <v>86</v>
       </c>
@@ -2766,9 +2714,9 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="45.6">
-      <c r="B5" s="102"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
+      <c r="B5" s="110"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
       <c r="E5" s="36" t="s">
         <v>89</v>
       </c>
@@ -2777,9 +2725,9 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="22.8">
-      <c r="B6" s="103"/>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
+      <c r="B6" s="111"/>
+      <c r="C6" s="108"/>
+      <c r="D6" s="108"/>
       <c r="E6" s="36" t="s">
         <v>91</v>
       </c>
@@ -2788,13 +2736,13 @@
       </c>
     </row>
     <row r="7" spans="2:6" ht="22.8">
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="109" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="98" t="s">
+      <c r="C7" s="106" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="98" t="s">
+      <c r="D7" s="106" t="s">
         <v>85</v>
       </c>
       <c r="E7" s="36" t="s">
@@ -2805,9 +2753,9 @@
       </c>
     </row>
     <row r="8" spans="2:6" ht="22.8">
-      <c r="B8" s="102"/>
-      <c r="C8" s="99"/>
-      <c r="D8" s="99"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
       <c r="E8" s="36" t="s">
         <v>86</v>
       </c>
@@ -2816,9 +2764,9 @@
       </c>
     </row>
     <row r="9" spans="2:6" ht="45.6">
-      <c r="B9" s="102"/>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
+      <c r="B9" s="110"/>
+      <c r="C9" s="107"/>
+      <c r="D9" s="107"/>
       <c r="E9" s="36" t="s">
         <v>89</v>
       </c>
@@ -2827,9 +2775,9 @@
       </c>
     </row>
     <row r="10" spans="2:6" ht="22.8">
-      <c r="B10" s="103"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
+      <c r="B10" s="111"/>
+      <c r="C10" s="108"/>
+      <c r="D10" s="108"/>
       <c r="E10" s="36" t="s">
         <v>91</v>
       </c>
@@ -2838,13 +2786,13 @@
       </c>
     </row>
     <row r="11" spans="2:6" ht="22.8">
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="109" t="s">
         <v>104</v>
       </c>
-      <c r="C11" s="98" t="s">
+      <c r="C11" s="106" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="98" t="s">
+      <c r="D11" s="106" t="s">
         <v>85</v>
       </c>
       <c r="E11" s="36" t="s">
@@ -2855,9 +2803,9 @@
       </c>
     </row>
     <row r="12" spans="2:6" ht="22.8">
-      <c r="B12" s="102"/>
-      <c r="C12" s="99"/>
-      <c r="D12" s="99"/>
+      <c r="B12" s="110"/>
+      <c r="C12" s="107"/>
+      <c r="D12" s="107"/>
       <c r="E12" s="36" t="s">
         <v>86</v>
       </c>
@@ -2866,9 +2814,9 @@
       </c>
     </row>
     <row r="13" spans="2:6" ht="45.6">
-      <c r="B13" s="102"/>
-      <c r="C13" s="99"/>
-      <c r="D13" s="99"/>
+      <c r="B13" s="110"/>
+      <c r="C13" s="107"/>
+      <c r="D13" s="107"/>
       <c r="E13" s="36" t="s">
         <v>89</v>
       </c>
@@ -2877,9 +2825,9 @@
       </c>
     </row>
     <row r="14" spans="2:6" ht="22.8">
-      <c r="B14" s="103"/>
-      <c r="C14" s="100"/>
-      <c r="D14" s="100"/>
+      <c r="B14" s="111"/>
+      <c r="C14" s="108"/>
+      <c r="D14" s="108"/>
       <c r="E14" s="36" t="s">
         <v>91</v>
       </c>
@@ -2888,13 +2836,13 @@
       </c>
     </row>
     <row r="15" spans="2:6" ht="22.8" customHeight="1">
-      <c r="B15" s="104" t="s">
+      <c r="B15" s="102" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="106" t="s">
+      <c r="C15" s="104" t="s">
         <v>106</v>
       </c>
-      <c r="D15" s="106" t="s">
+      <c r="D15" s="104" t="s">
         <v>94</v>
       </c>
       <c r="E15" s="37" t="s">
@@ -2905,9 +2853,9 @@
       </c>
     </row>
     <row r="16" spans="2:6" ht="22.8">
-      <c r="B16" s="105"/>
-      <c r="C16" s="107"/>
-      <c r="D16" s="107"/>
+      <c r="B16" s="103"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="105"/>
       <c r="E16" s="37" t="s">
         <v>96</v>
       </c>
@@ -2916,13 +2864,13 @@
       </c>
     </row>
     <row r="17" spans="2:6" ht="22.8">
-      <c r="B17" s="104" t="s">
+      <c r="B17" s="102" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="106" t="s">
+      <c r="C17" s="104" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="106" t="s">
+      <c r="D17" s="104" t="s">
         <v>94</v>
       </c>
       <c r="E17" s="37" t="s">
@@ -2933,9 +2881,9 @@
       </c>
     </row>
     <row r="18" spans="2:6" ht="22.8">
-      <c r="B18" s="105"/>
-      <c r="C18" s="107"/>
-      <c r="D18" s="107"/>
+      <c r="B18" s="103"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="105"/>
       <c r="E18" s="37" t="s">
         <v>96</v>
       </c>
@@ -2944,13 +2892,13 @@
       </c>
     </row>
     <row r="19" spans="2:6" ht="22.8">
-      <c r="B19" s="104" t="s">
+      <c r="B19" s="102" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="106" t="s">
+      <c r="C19" s="104" t="s">
         <v>101</v>
       </c>
-      <c r="D19" s="106" t="s">
+      <c r="D19" s="104" t="s">
         <v>94</v>
       </c>
       <c r="E19" s="37" t="s">
@@ -2961,9 +2909,9 @@
       </c>
     </row>
     <row r="20" spans="2:6" ht="22.8">
-      <c r="B20" s="105"/>
-      <c r="C20" s="107"/>
-      <c r="D20" s="107"/>
+      <c r="B20" s="103"/>
+      <c r="C20" s="105"/>
+      <c r="D20" s="105"/>
       <c r="E20" s="37" t="s">
         <v>96</v>
       </c>
@@ -2973,12 +2921,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="C3:C6"/>
     <mergeCell ref="B3:B6"/>
@@ -2991,6 +2933,12 @@
     <mergeCell ref="B11:B14"/>
     <mergeCell ref="C11:C14"/>
     <mergeCell ref="D11:D14"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3299,55 +3247,55 @@
       <c r="B6" s="3"/>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
-      <c r="E6" s="162" t="s">
+      <c r="E6" s="112" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="162"/>
-      <c r="G6" s="162"/>
-      <c r="H6" s="162"/>
-      <c r="I6" s="162"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
+      <c r="H6" s="112"/>
+      <c r="I6" s="112"/>
       <c r="J6" s="53"/>
       <c r="K6" s="49"/>
       <c r="L6" s="48"/>
-      <c r="M6" s="141" t="s">
+      <c r="M6" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="N6" s="141"/>
-      <c r="O6" s="141"/>
-      <c r="P6" s="141"/>
-      <c r="Q6" s="141"/>
-      <c r="R6" s="141"/>
-      <c r="S6" s="141"/>
-      <c r="T6" s="141"/>
-      <c r="U6" s="141" t="s">
+      <c r="N6" s="113"/>
+      <c r="O6" s="113"/>
+      <c r="P6" s="113"/>
+      <c r="Q6" s="113"/>
+      <c r="R6" s="113"/>
+      <c r="S6" s="113"/>
+      <c r="T6" s="113"/>
+      <c r="U6" s="113" t="s">
         <v>57</v>
       </c>
-      <c r="V6" s="141"/>
-      <c r="W6" s="141"/>
-      <c r="X6" s="141"/>
-      <c r="Y6" s="141"/>
-      <c r="Z6" s="141"/>
-      <c r="AA6" s="141"/>
-      <c r="AB6" s="141"/>
-      <c r="AC6" s="141" t="s">
+      <c r="V6" s="113"/>
+      <c r="W6" s="113"/>
+      <c r="X6" s="113"/>
+      <c r="Y6" s="113"/>
+      <c r="Z6" s="113"/>
+      <c r="AA6" s="113"/>
+      <c r="AB6" s="113"/>
+      <c r="AC6" s="113" t="s">
         <v>57</v>
       </c>
-      <c r="AD6" s="141"/>
-      <c r="AE6" s="141"/>
-      <c r="AF6" s="141"/>
-      <c r="AG6" s="141"/>
+      <c r="AD6" s="113"/>
+      <c r="AE6" s="113"/>
+      <c r="AF6" s="113"/>
+      <c r="AG6" s="113"/>
       <c r="AH6" s="53"/>
       <c r="AI6" s="49"/>
       <c r="AJ6" s="49"/>
       <c r="AK6" s="49"/>
       <c r="AL6" s="48"/>
-      <c r="AM6" s="163" t="s">
+      <c r="AM6" s="114" t="s">
         <v>58</v>
       </c>
-      <c r="AN6" s="163"/>
-      <c r="AO6" s="163"/>
-      <c r="AP6" s="163"/>
-      <c r="AQ6" s="163"/>
+      <c r="AN6" s="114"/>
+      <c r="AO6" s="114"/>
+      <c r="AP6" s="114"/>
+      <c r="AQ6" s="114"/>
       <c r="AR6" s="53"/>
       <c r="AS6" s="53"/>
       <c r="AT6" s="47"/>
@@ -3357,35 +3305,35 @@
       <c r="B7" s="3"/>
       <c r="C7" s="48"/>
       <c r="D7" s="48"/>
-      <c r="E7" s="162"/>
-      <c r="F7" s="162"/>
-      <c r="G7" s="162"/>
-      <c r="H7" s="162"/>
-      <c r="I7" s="162"/>
+      <c r="E7" s="112"/>
+      <c r="F7" s="112"/>
+      <c r="G7" s="112"/>
+      <c r="H7" s="112"/>
+      <c r="I7" s="112"/>
       <c r="J7" s="53"/>
       <c r="K7" s="54"/>
       <c r="L7" s="48"/>
-      <c r="M7" s="141"/>
-      <c r="N7" s="141"/>
-      <c r="O7" s="141"/>
-      <c r="P7" s="141"/>
-      <c r="Q7" s="141"/>
-      <c r="R7" s="141"/>
-      <c r="S7" s="141"/>
-      <c r="T7" s="141"/>
-      <c r="U7" s="141"/>
-      <c r="V7" s="141"/>
-      <c r="W7" s="141"/>
-      <c r="X7" s="141"/>
-      <c r="Y7" s="141"/>
-      <c r="Z7" s="141"/>
-      <c r="AA7" s="141"/>
-      <c r="AB7" s="141"/>
-      <c r="AC7" s="141"/>
-      <c r="AD7" s="141"/>
-      <c r="AE7" s="141"/>
-      <c r="AF7" s="141"/>
-      <c r="AG7" s="141"/>
+      <c r="M7" s="113"/>
+      <c r="N7" s="113"/>
+      <c r="O7" s="113"/>
+      <c r="P7" s="113"/>
+      <c r="Q7" s="113"/>
+      <c r="R7" s="113"/>
+      <c r="S7" s="113"/>
+      <c r="T7" s="113"/>
+      <c r="U7" s="113"/>
+      <c r="V7" s="113"/>
+      <c r="W7" s="113"/>
+      <c r="X7" s="113"/>
+      <c r="Y7" s="113"/>
+      <c r="Z7" s="113"/>
+      <c r="AA7" s="113"/>
+      <c r="AB7" s="113"/>
+      <c r="AC7" s="113"/>
+      <c r="AD7" s="113"/>
+      <c r="AE7" s="113"/>
+      <c r="AF7" s="113"/>
+      <c r="AG7" s="113"/>
       <c r="AH7" s="53"/>
       <c r="AI7" s="54"/>
       <c r="AJ7" s="55" t="s">
@@ -3393,11 +3341,11 @@
       </c>
       <c r="AK7" s="54"/>
       <c r="AL7" s="48"/>
-      <c r="AM7" s="163"/>
-      <c r="AN7" s="163"/>
-      <c r="AO7" s="163"/>
-      <c r="AP7" s="163"/>
-      <c r="AQ7" s="163"/>
+      <c r="AM7" s="114"/>
+      <c r="AN7" s="114"/>
+      <c r="AO7" s="114"/>
+      <c r="AP7" s="114"/>
+      <c r="AQ7" s="114"/>
       <c r="AR7" s="53"/>
       <c r="AS7" s="53"/>
       <c r="AT7" s="47"/>
@@ -3407,45 +3355,45 @@
       <c r="B8" s="3"/>
       <c r="C8" s="48"/>
       <c r="D8" s="48"/>
-      <c r="E8" s="162"/>
-      <c r="F8" s="162"/>
-      <c r="G8" s="162"/>
-      <c r="H8" s="162"/>
-      <c r="I8" s="162"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="112"/>
+      <c r="G8" s="112"/>
+      <c r="H8" s="112"/>
+      <c r="I8" s="112"/>
       <c r="J8" s="53"/>
       <c r="K8" s="49"/>
       <c r="L8" s="48"/>
-      <c r="M8" s="141"/>
-      <c r="N8" s="141"/>
-      <c r="O8" s="141"/>
-      <c r="P8" s="141"/>
-      <c r="Q8" s="141"/>
-      <c r="R8" s="141"/>
-      <c r="S8" s="141"/>
-      <c r="T8" s="141"/>
-      <c r="U8" s="141"/>
-      <c r="V8" s="141"/>
-      <c r="W8" s="141"/>
-      <c r="X8" s="141"/>
-      <c r="Y8" s="141"/>
-      <c r="Z8" s="141"/>
-      <c r="AA8" s="141"/>
-      <c r="AB8" s="141"/>
-      <c r="AC8" s="141"/>
-      <c r="AD8" s="141"/>
-      <c r="AE8" s="141"/>
-      <c r="AF8" s="141"/>
-      <c r="AG8" s="141"/>
+      <c r="M8" s="113"/>
+      <c r="N8" s="113"/>
+      <c r="O8" s="113"/>
+      <c r="P8" s="113"/>
+      <c r="Q8" s="113"/>
+      <c r="R8" s="113"/>
+      <c r="S8" s="113"/>
+      <c r="T8" s="113"/>
+      <c r="U8" s="113"/>
+      <c r="V8" s="113"/>
+      <c r="W8" s="113"/>
+      <c r="X8" s="113"/>
+      <c r="Y8" s="113"/>
+      <c r="Z8" s="113"/>
+      <c r="AA8" s="113"/>
+      <c r="AB8" s="113"/>
+      <c r="AC8" s="113"/>
+      <c r="AD8" s="113"/>
+      <c r="AE8" s="113"/>
+      <c r="AF8" s="113"/>
+      <c r="AG8" s="113"/>
       <c r="AH8" s="53"/>
       <c r="AI8" s="49"/>
       <c r="AJ8" s="49"/>
       <c r="AK8" s="49"/>
       <c r="AL8" s="48"/>
-      <c r="AM8" s="163"/>
-      <c r="AN8" s="163"/>
-      <c r="AO8" s="163"/>
-      <c r="AP8" s="163"/>
-      <c r="AQ8" s="163"/>
+      <c r="AM8" s="114"/>
+      <c r="AN8" s="114"/>
+      <c r="AO8" s="114"/>
+      <c r="AP8" s="114"/>
+      <c r="AQ8" s="114"/>
       <c r="AR8" s="53"/>
       <c r="AS8" s="53"/>
       <c r="AT8" s="47"/>
@@ -3455,47 +3403,47 @@
       <c r="B9" s="3"/>
       <c r="C9" s="48"/>
       <c r="D9" s="48"/>
-      <c r="E9" s="158" t="s">
+      <c r="E9" s="115" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="159"/>
+      <c r="F9" s="116"/>
       <c r="G9" s="49"/>
       <c r="H9" s="49"/>
       <c r="I9" s="49"/>
       <c r="J9" s="53"/>
       <c r="K9" s="49"/>
       <c r="L9" s="48"/>
-      <c r="M9" s="141"/>
-      <c r="N9" s="141"/>
-      <c r="O9" s="141"/>
-      <c r="P9" s="141"/>
-      <c r="Q9" s="141"/>
-      <c r="R9" s="141"/>
-      <c r="S9" s="141"/>
-      <c r="T9" s="141"/>
-      <c r="U9" s="141"/>
-      <c r="V9" s="141"/>
-      <c r="W9" s="141"/>
-      <c r="X9" s="141"/>
-      <c r="Y9" s="141"/>
-      <c r="Z9" s="141"/>
-      <c r="AA9" s="141"/>
-      <c r="AB9" s="141"/>
-      <c r="AC9" s="141"/>
-      <c r="AD9" s="141"/>
-      <c r="AE9" s="141"/>
-      <c r="AF9" s="141"/>
-      <c r="AG9" s="141"/>
+      <c r="M9" s="113"/>
+      <c r="N9" s="113"/>
+      <c r="O9" s="113"/>
+      <c r="P9" s="113"/>
+      <c r="Q9" s="113"/>
+      <c r="R9" s="113"/>
+      <c r="S9" s="113"/>
+      <c r="T9" s="113"/>
+      <c r="U9" s="113"/>
+      <c r="V9" s="113"/>
+      <c r="W9" s="113"/>
+      <c r="X9" s="113"/>
+      <c r="Y9" s="113"/>
+      <c r="Z9" s="113"/>
+      <c r="AA9" s="113"/>
+      <c r="AB9" s="113"/>
+      <c r="AC9" s="113"/>
+      <c r="AD9" s="113"/>
+      <c r="AE9" s="113"/>
+      <c r="AF9" s="113"/>
+      <c r="AG9" s="113"/>
       <c r="AH9" s="53"/>
       <c r="AI9" s="49"/>
       <c r="AJ9" s="49"/>
       <c r="AK9" s="49"/>
       <c r="AL9" s="48"/>
-      <c r="AM9" s="163"/>
-      <c r="AN9" s="163"/>
-      <c r="AO9" s="163"/>
-      <c r="AP9" s="163"/>
-      <c r="AQ9" s="163"/>
+      <c r="AM9" s="114"/>
+      <c r="AN9" s="114"/>
+      <c r="AO9" s="114"/>
+      <c r="AP9" s="114"/>
+      <c r="AQ9" s="114"/>
       <c r="AR9" s="53"/>
       <c r="AS9" s="53"/>
       <c r="AT9" s="47"/>
@@ -3505,8 +3453,8 @@
       <c r="B10" s="3"/>
       <c r="C10" s="48"/>
       <c r="D10" s="56"/>
-      <c r="E10" s="160"/>
-      <c r="F10" s="161"/>
+      <c r="E10" s="117"/>
+      <c r="F10" s="118"/>
       <c r="G10" s="57"/>
       <c r="H10" s="57"/>
       <c r="I10" s="57"/>
@@ -3652,10 +3600,10 @@
       <c r="E13" s="49"/>
       <c r="F13" s="59"/>
       <c r="G13" s="60"/>
-      <c r="H13" s="158" t="s">
+      <c r="H13" s="115" t="s">
         <v>60</v>
       </c>
-      <c r="I13" s="159"/>
+      <c r="I13" s="116"/>
       <c r="J13" s="49"/>
       <c r="K13" s="49"/>
       <c r="L13" s="49"/>
@@ -3702,50 +3650,50 @@
       <c r="E14" s="49"/>
       <c r="F14" s="59"/>
       <c r="G14" s="49"/>
-      <c r="H14" s="160"/>
-      <c r="I14" s="161"/>
+      <c r="H14" s="117"/>
+      <c r="I14" s="118"/>
       <c r="J14" s="49"/>
       <c r="K14" s="49"/>
       <c r="L14" s="49"/>
-      <c r="M14" s="164" t="s">
+      <c r="M14" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="N14" s="165"/>
-      <c r="O14" s="165"/>
-      <c r="P14" s="165"/>
-      <c r="Q14" s="166"/>
+      <c r="N14" s="120"/>
+      <c r="O14" s="120"/>
+      <c r="P14" s="120"/>
+      <c r="Q14" s="121"/>
       <c r="R14" s="49"/>
       <c r="S14" s="49"/>
       <c r="T14" s="49"/>
-      <c r="U14" s="164" t="s">
+      <c r="U14" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="V14" s="165"/>
-      <c r="W14" s="165"/>
-      <c r="X14" s="165"/>
-      <c r="Y14" s="166"/>
+      <c r="V14" s="120"/>
+      <c r="W14" s="120"/>
+      <c r="X14" s="120"/>
+      <c r="Y14" s="121"/>
       <c r="Z14" s="49"/>
       <c r="AA14" s="49"/>
       <c r="AB14" s="49"/>
-      <c r="AC14" s="164" t="s">
+      <c r="AC14" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="AD14" s="165"/>
-      <c r="AE14" s="165"/>
-      <c r="AF14" s="165"/>
-      <c r="AG14" s="166"/>
+      <c r="AD14" s="120"/>
+      <c r="AE14" s="120"/>
+      <c r="AF14" s="120"/>
+      <c r="AG14" s="121"/>
       <c r="AH14" s="49"/>
       <c r="AI14" s="49"/>
       <c r="AJ14" s="49"/>
       <c r="AK14" s="49"/>
       <c r="AL14" s="49"/>
-      <c r="AM14" s="164" t="s">
+      <c r="AM14" s="119" t="s">
         <v>109</v>
       </c>
-      <c r="AN14" s="165"/>
-      <c r="AO14" s="165"/>
-      <c r="AP14" s="165"/>
-      <c r="AQ14" s="166"/>
+      <c r="AN14" s="120"/>
+      <c r="AO14" s="120"/>
+      <c r="AP14" s="120"/>
+      <c r="AQ14" s="121"/>
       <c r="AR14" s="49"/>
       <c r="AS14" s="53"/>
       <c r="AT14" s="47"/>
@@ -3763,37 +3711,37 @@
       <c r="J15" s="49"/>
       <c r="K15" s="49"/>
       <c r="L15" s="49"/>
-      <c r="M15" s="167"/>
-      <c r="N15" s="168"/>
-      <c r="O15" s="168"/>
-      <c r="P15" s="168"/>
-      <c r="Q15" s="169"/>
+      <c r="M15" s="122"/>
+      <c r="N15" s="123"/>
+      <c r="O15" s="123"/>
+      <c r="P15" s="123"/>
+      <c r="Q15" s="124"/>
       <c r="R15" s="49"/>
       <c r="S15" s="49"/>
       <c r="T15" s="49"/>
-      <c r="U15" s="167"/>
-      <c r="V15" s="168"/>
-      <c r="W15" s="168"/>
-      <c r="X15" s="168"/>
-      <c r="Y15" s="169"/>
+      <c r="U15" s="122"/>
+      <c r="V15" s="123"/>
+      <c r="W15" s="123"/>
+      <c r="X15" s="123"/>
+      <c r="Y15" s="124"/>
       <c r="Z15" s="49"/>
       <c r="AA15" s="49"/>
       <c r="AB15" s="49"/>
-      <c r="AC15" s="167"/>
-      <c r="AD15" s="168"/>
-      <c r="AE15" s="168"/>
-      <c r="AF15" s="168"/>
-      <c r="AG15" s="169"/>
+      <c r="AC15" s="122"/>
+      <c r="AD15" s="123"/>
+      <c r="AE15" s="123"/>
+      <c r="AF15" s="123"/>
+      <c r="AG15" s="124"/>
       <c r="AH15" s="49"/>
       <c r="AI15" s="49"/>
       <c r="AJ15" s="49"/>
       <c r="AK15" s="49"/>
       <c r="AL15" s="49"/>
-      <c r="AM15" s="167"/>
-      <c r="AN15" s="168"/>
-      <c r="AO15" s="168"/>
-      <c r="AP15" s="168"/>
-      <c r="AQ15" s="169"/>
+      <c r="AM15" s="122"/>
+      <c r="AN15" s="123"/>
+      <c r="AO15" s="123"/>
+      <c r="AP15" s="123"/>
+      <c r="AQ15" s="124"/>
       <c r="AR15" s="49"/>
       <c r="AS15" s="53"/>
       <c r="AT15" s="47"/>
@@ -3803,15 +3751,15 @@
       <c r="B16" s="3"/>
       <c r="C16" s="48"/>
       <c r="D16" s="49"/>
-      <c r="E16" s="158" t="s">
+      <c r="E16" s="115" t="s">
         <v>62</v>
       </c>
-      <c r="F16" s="159"/>
+      <c r="F16" s="116"/>
       <c r="G16" s="49"/>
-      <c r="H16" s="158" t="s">
+      <c r="H16" s="115" t="s">
         <v>63</v>
       </c>
-      <c r="I16" s="159"/>
+      <c r="I16" s="116"/>
       <c r="J16" s="49"/>
       <c r="K16" s="49"/>
       <c r="L16" s="49"/>
@@ -3855,11 +3803,11 @@
       <c r="B17" s="3"/>
       <c r="C17" s="48"/>
       <c r="D17" s="49"/>
-      <c r="E17" s="160"/>
-      <c r="F17" s="161"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="118"/>
       <c r="G17" s="49"/>
-      <c r="H17" s="160"/>
-      <c r="I17" s="161"/>
+      <c r="H17" s="117"/>
+      <c r="I17" s="118"/>
       <c r="J17" s="49"/>
       <c r="K17" s="49"/>
       <c r="L17" s="49"/>
@@ -4009,40 +3957,40 @@
       <c r="B20" s="3"/>
       <c r="C20" s="48"/>
       <c r="D20" s="48"/>
-      <c r="E20" s="154" t="s">
+      <c r="E20" s="125" t="s">
         <v>69</v>
       </c>
-      <c r="F20" s="155"/>
+      <c r="F20" s="126"/>
       <c r="G20" s="49"/>
       <c r="H20" s="49"/>
       <c r="I20" s="49"/>
       <c r="J20" s="53"/>
       <c r="K20" s="49"/>
       <c r="L20" s="48"/>
-      <c r="M20" s="154" t="s">
+      <c r="M20" s="125" t="s">
         <v>69</v>
       </c>
-      <c r="N20" s="155"/>
+      <c r="N20" s="126"/>
       <c r="O20" s="49"/>
       <c r="P20" s="49"/>
       <c r="Q20" s="49"/>
       <c r="R20" s="53"/>
       <c r="S20" s="49"/>
       <c r="T20" s="48"/>
-      <c r="U20" s="154" t="s">
+      <c r="U20" s="125" t="s">
         <v>69</v>
       </c>
-      <c r="V20" s="155"/>
+      <c r="V20" s="126"/>
       <c r="W20" s="49"/>
       <c r="X20" s="49"/>
       <c r="Y20" s="49"/>
       <c r="Z20" s="53"/>
       <c r="AA20" s="49"/>
       <c r="AB20" s="48"/>
-      <c r="AC20" s="154" t="s">
+      <c r="AC20" s="125" t="s">
         <v>69</v>
       </c>
-      <c r="AD20" s="155"/>
+      <c r="AD20" s="126"/>
       <c r="AE20" s="49"/>
       <c r="AF20" s="49"/>
       <c r="AG20" s="49"/>
@@ -4051,10 +3999,10 @@
       <c r="AJ20" s="49"/>
       <c r="AK20" s="49"/>
       <c r="AL20" s="48"/>
-      <c r="AM20" s="154" t="s">
+      <c r="AM20" s="125" t="s">
         <v>69</v>
       </c>
-      <c r="AN20" s="155"/>
+      <c r="AN20" s="126"/>
       <c r="AO20" s="49"/>
       <c r="AP20" s="49"/>
       <c r="AQ20" s="49"/>
@@ -4067,55 +4015,55 @@
       <c r="B21" s="3"/>
       <c r="C21" s="48"/>
       <c r="D21" s="48"/>
-      <c r="E21" s="156"/>
-      <c r="F21" s="157"/>
+      <c r="E21" s="127"/>
+      <c r="F21" s="128"/>
       <c r="G21" s="49"/>
-      <c r="H21" s="154" t="s">
+      <c r="H21" s="125" t="s">
         <v>70</v>
       </c>
-      <c r="I21" s="155"/>
+      <c r="I21" s="126"/>
       <c r="J21" s="53"/>
       <c r="K21" s="49"/>
       <c r="L21" s="48"/>
-      <c r="M21" s="156"/>
-      <c r="N21" s="157"/>
+      <c r="M21" s="127"/>
+      <c r="N21" s="128"/>
       <c r="O21" s="49"/>
-      <c r="P21" s="154" t="s">
+      <c r="P21" s="125" t="s">
         <v>70</v>
       </c>
-      <c r="Q21" s="155"/>
+      <c r="Q21" s="126"/>
       <c r="R21" s="53"/>
       <c r="S21" s="49"/>
       <c r="T21" s="48"/>
-      <c r="U21" s="156"/>
-      <c r="V21" s="157"/>
+      <c r="U21" s="127"/>
+      <c r="V21" s="128"/>
       <c r="W21" s="49"/>
-      <c r="X21" s="154" t="s">
+      <c r="X21" s="125" t="s">
         <v>70</v>
       </c>
-      <c r="Y21" s="155"/>
+      <c r="Y21" s="126"/>
       <c r="Z21" s="53"/>
       <c r="AA21" s="49"/>
       <c r="AB21" s="48"/>
-      <c r="AC21" s="156"/>
-      <c r="AD21" s="157"/>
+      <c r="AC21" s="127"/>
+      <c r="AD21" s="128"/>
       <c r="AE21" s="49"/>
-      <c r="AF21" s="154" t="s">
+      <c r="AF21" s="125" t="s">
         <v>70</v>
       </c>
-      <c r="AG21" s="155"/>
+      <c r="AG21" s="126"/>
       <c r="AH21" s="53"/>
       <c r="AI21" s="49"/>
       <c r="AJ21" s="49"/>
       <c r="AK21" s="49"/>
       <c r="AL21" s="48"/>
-      <c r="AM21" s="156"/>
-      <c r="AN21" s="157"/>
+      <c r="AM21" s="127"/>
+      <c r="AN21" s="128"/>
       <c r="AO21" s="49"/>
-      <c r="AP21" s="154" t="s">
+      <c r="AP21" s="125" t="s">
         <v>70</v>
       </c>
-      <c r="AQ21" s="155"/>
+      <c r="AQ21" s="126"/>
       <c r="AR21" s="53"/>
       <c r="AS21" s="53"/>
       <c r="AT21" s="47"/>
@@ -4128,32 +4076,32 @@
       <c r="E22" s="49"/>
       <c r="F22" s="59"/>
       <c r="G22" s="49"/>
-      <c r="H22" s="156"/>
-      <c r="I22" s="157"/>
+      <c r="H22" s="127"/>
+      <c r="I22" s="128"/>
       <c r="J22" s="53"/>
       <c r="K22" s="49"/>
       <c r="L22" s="48"/>
       <c r="M22" s="49"/>
       <c r="N22" s="59"/>
       <c r="O22" s="49"/>
-      <c r="P22" s="156"/>
-      <c r="Q22" s="157"/>
+      <c r="P22" s="127"/>
+      <c r="Q22" s="128"/>
       <c r="R22" s="53"/>
       <c r="S22" s="49"/>
       <c r="T22" s="48"/>
       <c r="U22" s="49"/>
       <c r="V22" s="59"/>
       <c r="W22" s="49"/>
-      <c r="X22" s="156"/>
-      <c r="Y22" s="157"/>
+      <c r="X22" s="127"/>
+      <c r="Y22" s="128"/>
       <c r="Z22" s="53"/>
       <c r="AA22" s="49"/>
       <c r="AB22" s="48"/>
       <c r="AC22" s="49"/>
       <c r="AD22" s="59"/>
       <c r="AE22" s="49"/>
-      <c r="AF22" s="156"/>
-      <c r="AG22" s="157"/>
+      <c r="AF22" s="127"/>
+      <c r="AG22" s="128"/>
       <c r="AH22" s="53"/>
       <c r="AI22" s="49"/>
       <c r="AJ22" s="49"/>
@@ -4162,8 +4110,8 @@
       <c r="AM22" s="49"/>
       <c r="AN22" s="59"/>
       <c r="AO22" s="49"/>
-      <c r="AP22" s="156"/>
-      <c r="AQ22" s="157"/>
+      <c r="AP22" s="127"/>
+      <c r="AQ22" s="128"/>
       <c r="AR22" s="53"/>
       <c r="AS22" s="53"/>
       <c r="AT22" s="47"/>
@@ -4173,40 +4121,40 @@
       <c r="B23" s="3"/>
       <c r="C23" s="48"/>
       <c r="D23" s="48"/>
-      <c r="E23" s="154" t="s">
+      <c r="E23" s="125" t="s">
         <v>71</v>
       </c>
-      <c r="F23" s="155"/>
+      <c r="F23" s="126"/>
       <c r="G23" s="49"/>
       <c r="H23" s="50"/>
       <c r="I23" s="59"/>
       <c r="J23" s="53"/>
       <c r="K23" s="49"/>
       <c r="L23" s="48"/>
-      <c r="M23" s="154" t="s">
+      <c r="M23" s="125" t="s">
         <v>71</v>
       </c>
-      <c r="N23" s="155"/>
+      <c r="N23" s="126"/>
       <c r="O23" s="49"/>
       <c r="P23" s="50"/>
       <c r="Q23" s="66"/>
       <c r="R23" s="53"/>
       <c r="S23" s="49"/>
       <c r="T23" s="48"/>
-      <c r="U23" s="154" t="s">
+      <c r="U23" s="125" t="s">
         <v>71</v>
       </c>
-      <c r="V23" s="155"/>
+      <c r="V23" s="126"/>
       <c r="W23" s="49"/>
       <c r="X23" s="50"/>
       <c r="Y23" s="66"/>
       <c r="Z23" s="53"/>
       <c r="AA23" s="49"/>
       <c r="AB23" s="48"/>
-      <c r="AC23" s="154" t="s">
+      <c r="AC23" s="125" t="s">
         <v>71</v>
       </c>
-      <c r="AD23" s="155"/>
+      <c r="AD23" s="126"/>
       <c r="AE23" s="49"/>
       <c r="AF23" s="50"/>
       <c r="AG23" s="66"/>
@@ -4215,10 +4163,10 @@
       <c r="AJ23" s="49"/>
       <c r="AK23" s="49"/>
       <c r="AL23" s="48"/>
-      <c r="AM23" s="154" t="s">
+      <c r="AM23" s="125" t="s">
         <v>71</v>
       </c>
-      <c r="AN23" s="155"/>
+      <c r="AN23" s="126"/>
       <c r="AO23" s="49"/>
       <c r="AP23" s="50"/>
       <c r="AQ23" s="66"/>
@@ -4231,32 +4179,32 @@
       <c r="B24" s="3"/>
       <c r="C24" s="48"/>
       <c r="D24" s="48"/>
-      <c r="E24" s="156"/>
-      <c r="F24" s="157"/>
+      <c r="E24" s="127"/>
+      <c r="F24" s="128"/>
       <c r="G24" s="49"/>
       <c r="H24" s="49"/>
       <c r="I24" s="59"/>
       <c r="J24" s="53"/>
       <c r="K24" s="49"/>
       <c r="L24" s="48"/>
-      <c r="M24" s="156"/>
-      <c r="N24" s="157"/>
+      <c r="M24" s="127"/>
+      <c r="N24" s="128"/>
       <c r="O24" s="49"/>
       <c r="P24" s="49"/>
       <c r="Q24" s="59"/>
       <c r="R24" s="53"/>
       <c r="S24" s="49"/>
       <c r="T24" s="48"/>
-      <c r="U24" s="156"/>
-      <c r="V24" s="157"/>
+      <c r="U24" s="127"/>
+      <c r="V24" s="128"/>
       <c r="W24" s="49"/>
       <c r="X24" s="49"/>
       <c r="Y24" s="59"/>
       <c r="Z24" s="53"/>
       <c r="AA24" s="49"/>
       <c r="AB24" s="48"/>
-      <c r="AC24" s="156"/>
-      <c r="AD24" s="157"/>
+      <c r="AC24" s="127"/>
+      <c r="AD24" s="128"/>
       <c r="AE24" s="49"/>
       <c r="AF24" s="49"/>
       <c r="AG24" s="59"/>
@@ -4265,8 +4213,8 @@
       <c r="AJ24" s="49"/>
       <c r="AK24" s="49"/>
       <c r="AL24" s="48"/>
-      <c r="AM24" s="156"/>
-      <c r="AN24" s="157"/>
+      <c r="AM24" s="127"/>
+      <c r="AN24" s="128"/>
       <c r="AO24" s="49"/>
       <c r="AP24" s="49"/>
       <c r="AQ24" s="59"/>
@@ -4504,7 +4452,7 @@
       </c>
       <c r="AH29" s="54"/>
       <c r="AI29" s="48"/>
-      <c r="AJ29" s="141" t="s">
+      <c r="AJ29" s="113" t="s">
         <v>0</v>
       </c>
       <c r="AK29" s="53"/>
@@ -4556,7 +4504,7 @@
       </c>
       <c r="AH30" s="54"/>
       <c r="AI30" s="48"/>
-      <c r="AJ30" s="141"/>
+      <c r="AJ30" s="113"/>
       <c r="AK30" s="53"/>
       <c r="AL30" s="49"/>
       <c r="AM30" s="49"/>
@@ -4606,7 +4554,7 @@
       </c>
       <c r="AH31" s="54"/>
       <c r="AI31" s="48"/>
-      <c r="AJ31" s="141"/>
+      <c r="AJ31" s="113"/>
       <c r="AK31" s="53"/>
       <c r="AL31" s="54" t="s">
         <v>112</v>
@@ -4656,7 +4604,7 @@
       <c r="AG32" s="47"/>
       <c r="AH32" s="47"/>
       <c r="AI32" s="48"/>
-      <c r="AJ32" s="141"/>
+      <c r="AJ32" s="113"/>
       <c r="AK32" s="53"/>
       <c r="AL32" s="47"/>
       <c r="AM32" s="47"/>
@@ -4706,7 +4654,7 @@
       </c>
       <c r="AH33" s="54"/>
       <c r="AI33" s="48"/>
-      <c r="AJ33" s="141"/>
+      <c r="AJ33" s="113"/>
       <c r="AK33" s="53"/>
       <c r="AL33" s="47"/>
       <c r="AM33" s="47"/>
@@ -5022,36 +4970,36 @@
       <c r="M40" s="72"/>
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
-      <c r="P40" s="123" t="s">
+      <c r="P40" s="156" t="s">
         <v>119</v>
       </c>
-      <c r="Q40" s="124"/>
-      <c r="R40" s="124"/>
-      <c r="S40" s="124"/>
-      <c r="T40" s="124"/>
-      <c r="U40" s="125"/>
+      <c r="Q40" s="157"/>
+      <c r="R40" s="157"/>
+      <c r="S40" s="157"/>
+      <c r="T40" s="157"/>
+      <c r="U40" s="158"/>
       <c r="V40" s="77"/>
       <c r="W40" s="77"/>
-      <c r="X40" s="114" t="s">
+      <c r="X40" s="147" t="s">
         <v>73</v>
       </c>
-      <c r="Y40" s="115"/>
-      <c r="Z40" s="115"/>
-      <c r="AA40" s="115"/>
-      <c r="AB40" s="115"/>
-      <c r="AC40" s="116"/>
+      <c r="Y40" s="148"/>
+      <c r="Z40" s="148"/>
+      <c r="AA40" s="148"/>
+      <c r="AB40" s="148"/>
+      <c r="AC40" s="149"/>
       <c r="AD40" s="5"/>
       <c r="AE40" s="5"/>
-      <c r="AF40" s="142" t="s">
+      <c r="AF40" s="135" t="s">
         <v>114</v>
       </c>
-      <c r="AG40" s="143"/>
-      <c r="AH40" s="143"/>
-      <c r="AI40" s="143"/>
-      <c r="AJ40" s="143"/>
-      <c r="AK40" s="143"/>
-      <c r="AL40" s="143"/>
-      <c r="AM40" s="144"/>
+      <c r="AG40" s="136"/>
+      <c r="AH40" s="136"/>
+      <c r="AI40" s="136"/>
+      <c r="AJ40" s="136"/>
+      <c r="AK40" s="136"/>
+      <c r="AL40" s="136"/>
+      <c r="AM40" s="137"/>
       <c r="AN40" s="78"/>
       <c r="AO40" s="78"/>
       <c r="AP40" s="78"/>
@@ -5068,40 +5016,40 @@
       <c r="E41" s="73"/>
       <c r="F41" s="73"/>
       <c r="G41" s="4"/>
-      <c r="H41" s="108" t="s">
+      <c r="H41" s="141" t="s">
         <v>121</v>
       </c>
-      <c r="I41" s="109"/>
-      <c r="J41" s="109"/>
-      <c r="K41" s="109"/>
-      <c r="L41" s="109"/>
-      <c r="M41" s="110"/>
+      <c r="I41" s="142"/>
+      <c r="J41" s="142"/>
+      <c r="K41" s="142"/>
+      <c r="L41" s="142"/>
+      <c r="M41" s="143"/>
       <c r="N41" s="41"/>
       <c r="O41" s="42"/>
-      <c r="P41" s="126"/>
-      <c r="Q41" s="127"/>
-      <c r="R41" s="127"/>
-      <c r="S41" s="127"/>
-      <c r="T41" s="127"/>
-      <c r="U41" s="128"/>
+      <c r="P41" s="159"/>
+      <c r="Q41" s="160"/>
+      <c r="R41" s="160"/>
+      <c r="S41" s="160"/>
+      <c r="T41" s="160"/>
+      <c r="U41" s="161"/>
       <c r="V41" s="77"/>
       <c r="W41" s="77"/>
-      <c r="X41" s="117"/>
-      <c r="Y41" s="118"/>
-      <c r="Z41" s="118"/>
-      <c r="AA41" s="118"/>
-      <c r="AB41" s="118"/>
-      <c r="AC41" s="119"/>
+      <c r="X41" s="150"/>
+      <c r="Y41" s="151"/>
+      <c r="Z41" s="151"/>
+      <c r="AA41" s="151"/>
+      <c r="AB41" s="151"/>
+      <c r="AC41" s="152"/>
       <c r="AD41" s="3"/>
       <c r="AE41" s="3"/>
-      <c r="AF41" s="145"/>
-      <c r="AG41" s="146"/>
-      <c r="AH41" s="146"/>
-      <c r="AI41" s="146"/>
-      <c r="AJ41" s="146"/>
-      <c r="AK41" s="146"/>
-      <c r="AL41" s="146"/>
-      <c r="AM41" s="147"/>
+      <c r="AF41" s="138"/>
+      <c r="AG41" s="139"/>
+      <c r="AH41" s="139"/>
+      <c r="AI41" s="139"/>
+      <c r="AJ41" s="139"/>
+      <c r="AK41" s="139"/>
+      <c r="AL41" s="139"/>
+      <c r="AM41" s="140"/>
       <c r="AN41" s="78"/>
       <c r="AO41" s="78"/>
       <c r="AP41" s="78"/>
@@ -5118,28 +5066,28 @@
       <c r="E42" s="73"/>
       <c r="F42" s="73"/>
       <c r="G42" s="4"/>
-      <c r="H42" s="111"/>
-      <c r="I42" s="112"/>
-      <c r="J42" s="112"/>
-      <c r="K42" s="112"/>
-      <c r="L42" s="112"/>
-      <c r="M42" s="113"/>
+      <c r="H42" s="144"/>
+      <c r="I42" s="145"/>
+      <c r="J42" s="145"/>
+      <c r="K42" s="145"/>
+      <c r="L42" s="145"/>
+      <c r="M42" s="146"/>
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
-      <c r="P42" s="126"/>
-      <c r="Q42" s="127"/>
-      <c r="R42" s="127"/>
-      <c r="S42" s="127"/>
-      <c r="T42" s="127"/>
-      <c r="U42" s="128"/>
+      <c r="P42" s="159"/>
+      <c r="Q42" s="160"/>
+      <c r="R42" s="160"/>
+      <c r="S42" s="160"/>
+      <c r="T42" s="160"/>
+      <c r="U42" s="161"/>
       <c r="V42" s="76"/>
       <c r="W42" s="76"/>
-      <c r="X42" s="117"/>
-      <c r="Y42" s="118"/>
-      <c r="Z42" s="118"/>
-      <c r="AA42" s="118"/>
-      <c r="AB42" s="118"/>
-      <c r="AC42" s="119"/>
+      <c r="X42" s="150"/>
+      <c r="Y42" s="151"/>
+      <c r="Z42" s="151"/>
+      <c r="AA42" s="151"/>
+      <c r="AB42" s="151"/>
+      <c r="AC42" s="152"/>
       <c r="AD42" s="3"/>
       <c r="AE42" s="3"/>
       <c r="AF42" s="3"/>
@@ -5174,32 +5122,32 @@
       <c r="M43" s="72"/>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
-      <c r="P43" s="126"/>
-      <c r="Q43" s="127"/>
-      <c r="R43" s="127"/>
-      <c r="S43" s="127"/>
-      <c r="T43" s="127"/>
-      <c r="U43" s="128"/>
+      <c r="P43" s="159"/>
+      <c r="Q43" s="160"/>
+      <c r="R43" s="160"/>
+      <c r="S43" s="160"/>
+      <c r="T43" s="160"/>
+      <c r="U43" s="161"/>
       <c r="V43" s="80"/>
       <c r="W43" s="80"/>
-      <c r="X43" s="117"/>
-      <c r="Y43" s="118"/>
-      <c r="Z43" s="118"/>
-      <c r="AA43" s="118"/>
-      <c r="AB43" s="118"/>
-      <c r="AC43" s="119"/>
+      <c r="X43" s="150"/>
+      <c r="Y43" s="151"/>
+      <c r="Z43" s="151"/>
+      <c r="AA43" s="151"/>
+      <c r="AB43" s="151"/>
+      <c r="AC43" s="152"/>
       <c r="AD43" s="5"/>
       <c r="AE43" s="5"/>
-      <c r="AF43" s="142" t="s">
+      <c r="AF43" s="135" t="s">
         <v>115</v>
       </c>
-      <c r="AG43" s="143"/>
-      <c r="AH43" s="143"/>
-      <c r="AI43" s="143"/>
-      <c r="AJ43" s="143"/>
-      <c r="AK43" s="143"/>
-      <c r="AL43" s="143"/>
-      <c r="AM43" s="144"/>
+      <c r="AG43" s="136"/>
+      <c r="AH43" s="136"/>
+      <c r="AI43" s="136"/>
+      <c r="AJ43" s="136"/>
+      <c r="AK43" s="136"/>
+      <c r="AL43" s="136"/>
+      <c r="AM43" s="137"/>
       <c r="AN43" s="78"/>
       <c r="AO43" s="78"/>
       <c r="AP43" s="78"/>
@@ -5216,40 +5164,40 @@
       <c r="E44" s="73"/>
       <c r="F44" s="73"/>
       <c r="G44" s="4"/>
-      <c r="H44" s="108" t="s">
+      <c r="H44" s="141" t="s">
         <v>123</v>
       </c>
-      <c r="I44" s="109"/>
-      <c r="J44" s="109"/>
-      <c r="K44" s="109"/>
-      <c r="L44" s="109"/>
-      <c r="M44" s="110"/>
+      <c r="I44" s="142"/>
+      <c r="J44" s="142"/>
+      <c r="K44" s="142"/>
+      <c r="L44" s="142"/>
+      <c r="M44" s="143"/>
       <c r="N44" s="41"/>
       <c r="O44" s="42"/>
-      <c r="P44" s="126"/>
-      <c r="Q44" s="127"/>
-      <c r="R44" s="127"/>
-      <c r="S44" s="127"/>
-      <c r="T44" s="127"/>
-      <c r="U44" s="128"/>
+      <c r="P44" s="159"/>
+      <c r="Q44" s="160"/>
+      <c r="R44" s="160"/>
+      <c r="S44" s="160"/>
+      <c r="T44" s="160"/>
+      <c r="U44" s="161"/>
       <c r="V44" s="76"/>
       <c r="W44" s="76"/>
-      <c r="X44" s="117"/>
-      <c r="Y44" s="118"/>
-      <c r="Z44" s="118"/>
-      <c r="AA44" s="118"/>
-      <c r="AB44" s="118"/>
-      <c r="AC44" s="119"/>
+      <c r="X44" s="150"/>
+      <c r="Y44" s="151"/>
+      <c r="Z44" s="151"/>
+      <c r="AA44" s="151"/>
+      <c r="AB44" s="151"/>
+      <c r="AC44" s="152"/>
       <c r="AD44" s="3"/>
       <c r="AE44" s="3"/>
-      <c r="AF44" s="145"/>
-      <c r="AG44" s="146"/>
-      <c r="AH44" s="146"/>
-      <c r="AI44" s="146"/>
-      <c r="AJ44" s="146"/>
-      <c r="AK44" s="146"/>
-      <c r="AL44" s="146"/>
-      <c r="AM44" s="147"/>
+      <c r="AF44" s="138"/>
+      <c r="AG44" s="139"/>
+      <c r="AH44" s="139"/>
+      <c r="AI44" s="139"/>
+      <c r="AJ44" s="139"/>
+      <c r="AK44" s="139"/>
+      <c r="AL44" s="139"/>
+      <c r="AM44" s="140"/>
       <c r="AN44" s="78"/>
       <c r="AO44" s="78"/>
       <c r="AP44" s="78"/>
@@ -5266,28 +5214,28 @@
       <c r="E45" s="73"/>
       <c r="F45" s="73"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="111"/>
-      <c r="I45" s="112"/>
-      <c r="J45" s="112"/>
-      <c r="K45" s="112"/>
-      <c r="L45" s="112"/>
-      <c r="M45" s="113"/>
+      <c r="H45" s="144"/>
+      <c r="I45" s="145"/>
+      <c r="J45" s="145"/>
+      <c r="K45" s="145"/>
+      <c r="L45" s="145"/>
+      <c r="M45" s="146"/>
       <c r="N45" s="4"/>
       <c r="O45" s="4"/>
-      <c r="P45" s="126"/>
-      <c r="Q45" s="127"/>
-      <c r="R45" s="127"/>
-      <c r="S45" s="127"/>
-      <c r="T45" s="127"/>
-      <c r="U45" s="128"/>
+      <c r="P45" s="159"/>
+      <c r="Q45" s="160"/>
+      <c r="R45" s="160"/>
+      <c r="S45" s="160"/>
+      <c r="T45" s="160"/>
+      <c r="U45" s="161"/>
       <c r="V45" s="81"/>
       <c r="W45" s="81"/>
-      <c r="X45" s="117"/>
-      <c r="Y45" s="118"/>
-      <c r="Z45" s="118"/>
-      <c r="AA45" s="118"/>
-      <c r="AB45" s="118"/>
-      <c r="AC45" s="119"/>
+      <c r="X45" s="150"/>
+      <c r="Y45" s="151"/>
+      <c r="Z45" s="151"/>
+      <c r="AA45" s="151"/>
+      <c r="AB45" s="151"/>
+      <c r="AC45" s="152"/>
       <c r="AD45" s="3"/>
       <c r="AE45" s="3"/>
       <c r="AF45" s="3"/>
@@ -5322,32 +5270,32 @@
       <c r="M46" s="72"/>
       <c r="N46" s="4"/>
       <c r="O46" s="4"/>
-      <c r="P46" s="126"/>
-      <c r="Q46" s="127"/>
-      <c r="R46" s="127"/>
-      <c r="S46" s="127"/>
-      <c r="T46" s="127"/>
-      <c r="U46" s="128"/>
+      <c r="P46" s="159"/>
+      <c r="Q46" s="160"/>
+      <c r="R46" s="160"/>
+      <c r="S46" s="160"/>
+      <c r="T46" s="160"/>
+      <c r="U46" s="161"/>
       <c r="V46" s="77"/>
       <c r="W46" s="77"/>
-      <c r="X46" s="117"/>
-      <c r="Y46" s="118"/>
-      <c r="Z46" s="118"/>
-      <c r="AA46" s="118"/>
-      <c r="AB46" s="118"/>
-      <c r="AC46" s="119"/>
+      <c r="X46" s="150"/>
+      <c r="Y46" s="151"/>
+      <c r="Z46" s="151"/>
+      <c r="AA46" s="151"/>
+      <c r="AB46" s="151"/>
+      <c r="AC46" s="152"/>
       <c r="AD46" s="5"/>
       <c r="AE46" s="5"/>
-      <c r="AF46" s="142" t="s">
+      <c r="AF46" s="135" t="s">
         <v>116</v>
       </c>
-      <c r="AG46" s="143"/>
-      <c r="AH46" s="143"/>
-      <c r="AI46" s="143"/>
-      <c r="AJ46" s="143"/>
-      <c r="AK46" s="143"/>
-      <c r="AL46" s="143"/>
-      <c r="AM46" s="144"/>
+      <c r="AG46" s="136"/>
+      <c r="AH46" s="136"/>
+      <c r="AI46" s="136"/>
+      <c r="AJ46" s="136"/>
+      <c r="AK46" s="136"/>
+      <c r="AL46" s="136"/>
+      <c r="AM46" s="137"/>
       <c r="AN46" s="78"/>
       <c r="AO46" s="78"/>
       <c r="AP46" s="78"/>
@@ -5364,40 +5312,40 @@
       <c r="E47" s="73"/>
       <c r="F47" s="73"/>
       <c r="G47" s="4"/>
-      <c r="H47" s="108" t="s">
+      <c r="H47" s="141" t="s">
         <v>124</v>
       </c>
-      <c r="I47" s="109"/>
-      <c r="J47" s="109"/>
-      <c r="K47" s="109"/>
-      <c r="L47" s="109"/>
-      <c r="M47" s="110"/>
+      <c r="I47" s="142"/>
+      <c r="J47" s="142"/>
+      <c r="K47" s="142"/>
+      <c r="L47" s="142"/>
+      <c r="M47" s="143"/>
       <c r="N47" s="41"/>
       <c r="O47" s="42"/>
-      <c r="P47" s="126"/>
-      <c r="Q47" s="127"/>
-      <c r="R47" s="127"/>
-      <c r="S47" s="127"/>
-      <c r="T47" s="127"/>
-      <c r="U47" s="128"/>
+      <c r="P47" s="159"/>
+      <c r="Q47" s="160"/>
+      <c r="R47" s="160"/>
+      <c r="S47" s="160"/>
+      <c r="T47" s="160"/>
+      <c r="U47" s="161"/>
       <c r="V47" s="77"/>
       <c r="W47" s="77"/>
-      <c r="X47" s="117"/>
-      <c r="Y47" s="118"/>
-      <c r="Z47" s="118"/>
-      <c r="AA47" s="118"/>
-      <c r="AB47" s="118"/>
-      <c r="AC47" s="119"/>
+      <c r="X47" s="150"/>
+      <c r="Y47" s="151"/>
+      <c r="Z47" s="151"/>
+      <c r="AA47" s="151"/>
+      <c r="AB47" s="151"/>
+      <c r="AC47" s="152"/>
       <c r="AD47" s="3"/>
       <c r="AE47" s="3"/>
-      <c r="AF47" s="145"/>
-      <c r="AG47" s="146"/>
-      <c r="AH47" s="146"/>
-      <c r="AI47" s="146"/>
-      <c r="AJ47" s="146"/>
-      <c r="AK47" s="146"/>
-      <c r="AL47" s="146"/>
-      <c r="AM47" s="147"/>
+      <c r="AF47" s="138"/>
+      <c r="AG47" s="139"/>
+      <c r="AH47" s="139"/>
+      <c r="AI47" s="139"/>
+      <c r="AJ47" s="139"/>
+      <c r="AK47" s="139"/>
+      <c r="AL47" s="139"/>
+      <c r="AM47" s="140"/>
       <c r="AN47" s="78"/>
       <c r="AO47" s="78"/>
       <c r="AP47" s="78"/>
@@ -5414,28 +5362,28 @@
       <c r="E48" s="73"/>
       <c r="F48" s="73"/>
       <c r="G48" s="4"/>
-      <c r="H48" s="111"/>
-      <c r="I48" s="112"/>
-      <c r="J48" s="112"/>
-      <c r="K48" s="112"/>
-      <c r="L48" s="112"/>
-      <c r="M48" s="113"/>
+      <c r="H48" s="144"/>
+      <c r="I48" s="145"/>
+      <c r="J48" s="145"/>
+      <c r="K48" s="145"/>
+      <c r="L48" s="145"/>
+      <c r="M48" s="146"/>
       <c r="N48" s="4"/>
       <c r="O48" s="4"/>
-      <c r="P48" s="126"/>
-      <c r="Q48" s="127"/>
-      <c r="R48" s="127"/>
-      <c r="S48" s="127"/>
-      <c r="T48" s="127"/>
-      <c r="U48" s="128"/>
+      <c r="P48" s="159"/>
+      <c r="Q48" s="160"/>
+      <c r="R48" s="160"/>
+      <c r="S48" s="160"/>
+      <c r="T48" s="160"/>
+      <c r="U48" s="161"/>
       <c r="V48" s="76"/>
       <c r="W48" s="76"/>
-      <c r="X48" s="117"/>
-      <c r="Y48" s="118"/>
-      <c r="Z48" s="118"/>
-      <c r="AA48" s="118"/>
-      <c r="AB48" s="118"/>
-      <c r="AC48" s="119"/>
+      <c r="X48" s="150"/>
+      <c r="Y48" s="151"/>
+      <c r="Z48" s="151"/>
+      <c r="AA48" s="151"/>
+      <c r="AB48" s="151"/>
+      <c r="AC48" s="152"/>
       <c r="AD48" s="3"/>
       <c r="AE48" s="3"/>
       <c r="AF48" s="3"/>
@@ -5470,32 +5418,32 @@
       <c r="M49" s="72"/>
       <c r="N49" s="4"/>
       <c r="O49" s="4"/>
-      <c r="P49" s="126"/>
-      <c r="Q49" s="127"/>
-      <c r="R49" s="127"/>
-      <c r="S49" s="127"/>
-      <c r="T49" s="127"/>
-      <c r="U49" s="128"/>
+      <c r="P49" s="159"/>
+      <c r="Q49" s="160"/>
+      <c r="R49" s="160"/>
+      <c r="S49" s="160"/>
+      <c r="T49" s="160"/>
+      <c r="U49" s="161"/>
       <c r="V49" s="77"/>
       <c r="W49" s="77"/>
-      <c r="X49" s="117"/>
-      <c r="Y49" s="118"/>
-      <c r="Z49" s="118"/>
-      <c r="AA49" s="118"/>
-      <c r="AB49" s="118"/>
-      <c r="AC49" s="119"/>
+      <c r="X49" s="150"/>
+      <c r="Y49" s="151"/>
+      <c r="Z49" s="151"/>
+      <c r="AA49" s="151"/>
+      <c r="AB49" s="151"/>
+      <c r="AC49" s="152"/>
       <c r="AD49" s="5"/>
       <c r="AE49" s="5"/>
-      <c r="AF49" s="148" t="s">
+      <c r="AF49" s="129" t="s">
         <v>118</v>
       </c>
-      <c r="AG49" s="149"/>
-      <c r="AH49" s="149"/>
-      <c r="AI49" s="149"/>
-      <c r="AJ49" s="149"/>
-      <c r="AK49" s="149"/>
-      <c r="AL49" s="149"/>
-      <c r="AM49" s="150"/>
+      <c r="AG49" s="130"/>
+      <c r="AH49" s="130"/>
+      <c r="AI49" s="130"/>
+      <c r="AJ49" s="130"/>
+      <c r="AK49" s="130"/>
+      <c r="AL49" s="130"/>
+      <c r="AM49" s="131"/>
       <c r="AN49" s="78"/>
       <c r="AO49" s="78"/>
       <c r="AP49" s="78"/>
@@ -5520,30 +5468,30 @@
       <c r="M50" s="72"/>
       <c r="N50" s="4"/>
       <c r="O50" s="4"/>
-      <c r="P50" s="129"/>
-      <c r="Q50" s="130"/>
-      <c r="R50" s="130"/>
-      <c r="S50" s="130"/>
-      <c r="T50" s="130"/>
-      <c r="U50" s="131"/>
+      <c r="P50" s="162"/>
+      <c r="Q50" s="163"/>
+      <c r="R50" s="163"/>
+      <c r="S50" s="163"/>
+      <c r="T50" s="163"/>
+      <c r="U50" s="164"/>
       <c r="V50" s="76"/>
       <c r="W50" s="76"/>
-      <c r="X50" s="117"/>
-      <c r="Y50" s="118"/>
-      <c r="Z50" s="118"/>
-      <c r="AA50" s="118"/>
-      <c r="AB50" s="118"/>
-      <c r="AC50" s="119"/>
+      <c r="X50" s="150"/>
+      <c r="Y50" s="151"/>
+      <c r="Z50" s="151"/>
+      <c r="AA50" s="151"/>
+      <c r="AB50" s="151"/>
+      <c r="AC50" s="152"/>
       <c r="AD50" s="3"/>
       <c r="AE50" s="3"/>
-      <c r="AF50" s="151"/>
-      <c r="AG50" s="152"/>
-      <c r="AH50" s="152"/>
-      <c r="AI50" s="152"/>
-      <c r="AJ50" s="152"/>
-      <c r="AK50" s="152"/>
-      <c r="AL50" s="152"/>
-      <c r="AM50" s="153"/>
+      <c r="AF50" s="132"/>
+      <c r="AG50" s="133"/>
+      <c r="AH50" s="133"/>
+      <c r="AI50" s="133"/>
+      <c r="AJ50" s="133"/>
+      <c r="AK50" s="133"/>
+      <c r="AL50" s="133"/>
+      <c r="AM50" s="134"/>
       <c r="AN50" s="78"/>
       <c r="AO50" s="78"/>
       <c r="AP50" s="78"/>
@@ -5576,12 +5524,12 @@
       <c r="U51" s="82"/>
       <c r="V51" s="83"/>
       <c r="W51" s="77"/>
-      <c r="X51" s="117"/>
-      <c r="Y51" s="118"/>
-      <c r="Z51" s="118"/>
-      <c r="AA51" s="118"/>
-      <c r="AB51" s="118"/>
-      <c r="AC51" s="119"/>
+      <c r="X51" s="150"/>
+      <c r="Y51" s="151"/>
+      <c r="Z51" s="151"/>
+      <c r="AA51" s="151"/>
+      <c r="AB51" s="151"/>
+      <c r="AC51" s="152"/>
       <c r="AD51" s="3"/>
       <c r="AE51" s="3"/>
       <c r="AF51" s="3"/>
@@ -5616,34 +5564,34 @@
       <c r="M52" s="72"/>
       <c r="N52" s="4"/>
       <c r="O52" s="4"/>
-      <c r="P52" s="132" t="s">
+      <c r="P52" s="165" t="s">
         <v>120</v>
       </c>
-      <c r="Q52" s="133"/>
-      <c r="R52" s="133"/>
-      <c r="S52" s="133"/>
-      <c r="T52" s="133"/>
-      <c r="U52" s="134"/>
+      <c r="Q52" s="166"/>
+      <c r="R52" s="166"/>
+      <c r="S52" s="166"/>
+      <c r="T52" s="166"/>
+      <c r="U52" s="167"/>
       <c r="V52" s="77"/>
       <c r="W52" s="77"/>
-      <c r="X52" s="117"/>
-      <c r="Y52" s="118"/>
-      <c r="Z52" s="118"/>
-      <c r="AA52" s="118"/>
-      <c r="AB52" s="118"/>
-      <c r="AC52" s="119"/>
+      <c r="X52" s="150"/>
+      <c r="Y52" s="151"/>
+      <c r="Z52" s="151"/>
+      <c r="AA52" s="151"/>
+      <c r="AB52" s="151"/>
+      <c r="AC52" s="152"/>
       <c r="AD52" s="5"/>
       <c r="AE52" s="5"/>
-      <c r="AF52" s="148" t="s">
+      <c r="AF52" s="129" t="s">
         <v>117</v>
       </c>
-      <c r="AG52" s="149"/>
-      <c r="AH52" s="149"/>
-      <c r="AI52" s="149"/>
-      <c r="AJ52" s="149"/>
-      <c r="AK52" s="149"/>
-      <c r="AL52" s="149"/>
-      <c r="AM52" s="150"/>
+      <c r="AG52" s="130"/>
+      <c r="AH52" s="130"/>
+      <c r="AI52" s="130"/>
+      <c r="AJ52" s="130"/>
+      <c r="AK52" s="130"/>
+      <c r="AL52" s="130"/>
+      <c r="AM52" s="131"/>
       <c r="AN52" s="78"/>
       <c r="AO52" s="78"/>
       <c r="AP52" s="78"/>
@@ -5660,40 +5608,40 @@
       <c r="E53" s="73"/>
       <c r="F53" s="73"/>
       <c r="G53" s="4"/>
-      <c r="H53" s="108" t="s">
+      <c r="H53" s="141" t="s">
         <v>122</v>
       </c>
-      <c r="I53" s="109"/>
-      <c r="J53" s="109"/>
-      <c r="K53" s="109"/>
-      <c r="L53" s="109"/>
-      <c r="M53" s="110"/>
+      <c r="I53" s="142"/>
+      <c r="J53" s="142"/>
+      <c r="K53" s="142"/>
+      <c r="L53" s="142"/>
+      <c r="M53" s="143"/>
       <c r="N53" s="41"/>
       <c r="O53" s="42"/>
-      <c r="P53" s="135"/>
-      <c r="Q53" s="136"/>
-      <c r="R53" s="136"/>
-      <c r="S53" s="136"/>
-      <c r="T53" s="136"/>
-      <c r="U53" s="137"/>
+      <c r="P53" s="168"/>
+      <c r="Q53" s="169"/>
+      <c r="R53" s="169"/>
+      <c r="S53" s="169"/>
+      <c r="T53" s="169"/>
+      <c r="U53" s="170"/>
       <c r="V53" s="81"/>
       <c r="W53" s="81"/>
-      <c r="X53" s="117"/>
-      <c r="Y53" s="118"/>
-      <c r="Z53" s="118"/>
-      <c r="AA53" s="118"/>
-      <c r="AB53" s="118"/>
-      <c r="AC53" s="119"/>
+      <c r="X53" s="150"/>
+      <c r="Y53" s="151"/>
+      <c r="Z53" s="151"/>
+      <c r="AA53" s="151"/>
+      <c r="AB53" s="151"/>
+      <c r="AC53" s="152"/>
       <c r="AD53" s="3"/>
       <c r="AE53" s="3"/>
-      <c r="AF53" s="151"/>
-      <c r="AG53" s="152"/>
-      <c r="AH53" s="152"/>
-      <c r="AI53" s="152"/>
-      <c r="AJ53" s="152"/>
-      <c r="AK53" s="152"/>
-      <c r="AL53" s="152"/>
-      <c r="AM53" s="153"/>
+      <c r="AF53" s="132"/>
+      <c r="AG53" s="133"/>
+      <c r="AH53" s="133"/>
+      <c r="AI53" s="133"/>
+      <c r="AJ53" s="133"/>
+      <c r="AK53" s="133"/>
+      <c r="AL53" s="133"/>
+      <c r="AM53" s="134"/>
       <c r="AN53" s="78"/>
       <c r="AO53" s="78"/>
       <c r="AP53" s="78"/>
@@ -5710,28 +5658,28 @@
       <c r="E54" s="73"/>
       <c r="F54" s="73"/>
       <c r="G54" s="4"/>
-      <c r="H54" s="111"/>
-      <c r="I54" s="112"/>
-      <c r="J54" s="112"/>
-      <c r="K54" s="112"/>
-      <c r="L54" s="112"/>
-      <c r="M54" s="113"/>
+      <c r="H54" s="144"/>
+      <c r="I54" s="145"/>
+      <c r="J54" s="145"/>
+      <c r="K54" s="145"/>
+      <c r="L54" s="145"/>
+      <c r="M54" s="146"/>
       <c r="N54" s="4"/>
       <c r="O54" s="4"/>
-      <c r="P54" s="135"/>
-      <c r="Q54" s="136"/>
-      <c r="R54" s="136"/>
-      <c r="S54" s="136"/>
-      <c r="T54" s="136"/>
-      <c r="U54" s="137"/>
+      <c r="P54" s="168"/>
+      <c r="Q54" s="169"/>
+      <c r="R54" s="169"/>
+      <c r="S54" s="169"/>
+      <c r="T54" s="169"/>
+      <c r="U54" s="170"/>
       <c r="V54" s="77"/>
       <c r="W54" s="77"/>
-      <c r="X54" s="117"/>
-      <c r="Y54" s="118"/>
-      <c r="Z54" s="118"/>
-      <c r="AA54" s="118"/>
-      <c r="AB54" s="118"/>
-      <c r="AC54" s="119"/>
+      <c r="X54" s="150"/>
+      <c r="Y54" s="151"/>
+      <c r="Z54" s="151"/>
+      <c r="AA54" s="151"/>
+      <c r="AB54" s="151"/>
+      <c r="AC54" s="152"/>
       <c r="AD54" s="3"/>
       <c r="AE54" s="3"/>
       <c r="AF54" s="3"/>
@@ -5766,32 +5714,32 @@
       <c r="M55" s="72"/>
       <c r="N55" s="4"/>
       <c r="O55" s="4"/>
-      <c r="P55" s="135"/>
-      <c r="Q55" s="136"/>
-      <c r="R55" s="136"/>
-      <c r="S55" s="136"/>
-      <c r="T55" s="136"/>
-      <c r="U55" s="137"/>
+      <c r="P55" s="168"/>
+      <c r="Q55" s="169"/>
+      <c r="R55" s="169"/>
+      <c r="S55" s="169"/>
+      <c r="T55" s="169"/>
+      <c r="U55" s="170"/>
       <c r="V55" s="77"/>
       <c r="W55" s="77"/>
-      <c r="X55" s="117"/>
-      <c r="Y55" s="118"/>
-      <c r="Z55" s="118"/>
-      <c r="AA55" s="118"/>
-      <c r="AB55" s="118"/>
-      <c r="AC55" s="119"/>
+      <c r="X55" s="150"/>
+      <c r="Y55" s="151"/>
+      <c r="Z55" s="151"/>
+      <c r="AA55" s="151"/>
+      <c r="AB55" s="151"/>
+      <c r="AC55" s="152"/>
       <c r="AD55" s="5"/>
       <c r="AE55" s="5"/>
-      <c r="AF55" s="148" t="s">
+      <c r="AF55" s="129" t="s">
         <v>74</v>
       </c>
-      <c r="AG55" s="149"/>
-      <c r="AH55" s="149"/>
-      <c r="AI55" s="149"/>
-      <c r="AJ55" s="149"/>
-      <c r="AK55" s="149"/>
-      <c r="AL55" s="149"/>
-      <c r="AM55" s="150"/>
+      <c r="AG55" s="130"/>
+      <c r="AH55" s="130"/>
+      <c r="AI55" s="130"/>
+      <c r="AJ55" s="130"/>
+      <c r="AK55" s="130"/>
+      <c r="AL55" s="130"/>
+      <c r="AM55" s="131"/>
       <c r="AN55" s="78"/>
       <c r="AO55" s="78"/>
       <c r="AP55" s="78"/>
@@ -5816,30 +5764,30 @@
       <c r="M56" s="72"/>
       <c r="N56" s="4"/>
       <c r="O56" s="4"/>
-      <c r="P56" s="138"/>
-      <c r="Q56" s="139"/>
-      <c r="R56" s="139"/>
-      <c r="S56" s="139"/>
-      <c r="T56" s="139"/>
-      <c r="U56" s="140"/>
+      <c r="P56" s="171"/>
+      <c r="Q56" s="172"/>
+      <c r="R56" s="172"/>
+      <c r="S56" s="172"/>
+      <c r="T56" s="172"/>
+      <c r="U56" s="173"/>
       <c r="V56" s="77"/>
       <c r="W56" s="77"/>
-      <c r="X56" s="120"/>
-      <c r="Y56" s="121"/>
-      <c r="Z56" s="121"/>
-      <c r="AA56" s="121"/>
-      <c r="AB56" s="121"/>
-      <c r="AC56" s="122"/>
+      <c r="X56" s="153"/>
+      <c r="Y56" s="154"/>
+      <c r="Z56" s="154"/>
+      <c r="AA56" s="154"/>
+      <c r="AB56" s="154"/>
+      <c r="AC56" s="155"/>
       <c r="AD56" s="3"/>
       <c r="AE56" s="3"/>
-      <c r="AF56" s="151"/>
-      <c r="AG56" s="152"/>
-      <c r="AH56" s="152"/>
-      <c r="AI56" s="152"/>
-      <c r="AJ56" s="152"/>
-      <c r="AK56" s="152"/>
-      <c r="AL56" s="152"/>
-      <c r="AM56" s="153"/>
+      <c r="AF56" s="132"/>
+      <c r="AG56" s="133"/>
+      <c r="AH56" s="133"/>
+      <c r="AI56" s="133"/>
+      <c r="AJ56" s="133"/>
+      <c r="AK56" s="133"/>
+      <c r="AL56" s="133"/>
+      <c r="AM56" s="134"/>
       <c r="AN56" s="78"/>
       <c r="AO56" s="78"/>
       <c r="AP56" s="78"/>
@@ -5973,20 +5921,16 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E6:I8"/>
-    <mergeCell ref="M6:AG9"/>
-    <mergeCell ref="AM6:AQ9"/>
-    <mergeCell ref="E9:F10"/>
-    <mergeCell ref="H13:I14"/>
-    <mergeCell ref="M14:Q15"/>
-    <mergeCell ref="U14:Y15"/>
-    <mergeCell ref="AC14:AG15"/>
-    <mergeCell ref="AM14:AQ15"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="H16:I17"/>
-    <mergeCell ref="E20:F21"/>
-    <mergeCell ref="M20:N21"/>
-    <mergeCell ref="U20:V21"/>
+    <mergeCell ref="H53:M54"/>
+    <mergeCell ref="X40:AC56"/>
+    <mergeCell ref="P40:U50"/>
+    <mergeCell ref="P52:U56"/>
+    <mergeCell ref="AF43:AM44"/>
+    <mergeCell ref="AF46:AM47"/>
+    <mergeCell ref="AF49:AM50"/>
+    <mergeCell ref="H41:M42"/>
+    <mergeCell ref="H44:M45"/>
+    <mergeCell ref="H47:M48"/>
     <mergeCell ref="AF52:AM53"/>
     <mergeCell ref="AF55:AM56"/>
     <mergeCell ref="AP21:AQ22"/>
@@ -6003,20 +5947,24 @@
     <mergeCell ref="AF21:AG22"/>
     <mergeCell ref="AJ29:AJ33"/>
     <mergeCell ref="AF40:AM41"/>
-    <mergeCell ref="AF43:AM44"/>
-    <mergeCell ref="AF46:AM47"/>
-    <mergeCell ref="AF49:AM50"/>
-    <mergeCell ref="H41:M42"/>
-    <mergeCell ref="H44:M45"/>
-    <mergeCell ref="H47:M48"/>
-    <mergeCell ref="H53:M54"/>
-    <mergeCell ref="X40:AC56"/>
-    <mergeCell ref="P40:U50"/>
-    <mergeCell ref="P52:U56"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="H16:I17"/>
+    <mergeCell ref="E20:F21"/>
+    <mergeCell ref="M20:N21"/>
+    <mergeCell ref="U20:V21"/>
+    <mergeCell ref="E6:I8"/>
+    <mergeCell ref="M6:AG9"/>
+    <mergeCell ref="AM6:AQ9"/>
+    <mergeCell ref="E9:F10"/>
+    <mergeCell ref="H13:I14"/>
+    <mergeCell ref="M14:Q15"/>
+    <mergeCell ref="U14:Y15"/>
+    <mergeCell ref="AC14:AG15"/>
+    <mergeCell ref="AM14:AQ15"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12Page &amp;P</oddFooter>

</xml_diff>